<commit_message>
1.) Update the report excel template; 2.) Update the function to generate tradings.
</commit_message>
<xml_diff>
--- a/data/report/ARK.xlsx
+++ b/data/report/ARK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrick/go/src/github.com/skeyic/ark-robot/data/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15902\go\src\github.com\skeyic\ark-robot\data\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683FC8E7-7D00-2D44-9D43-A039D34A6C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB83C29C-20C6-4C75-8EE7-1C9815244A9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="22060" windowHeight="12360" xr2:uid="{F07BBE50-B47C-4F49-968F-328D3756EA4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F07BBE50-B47C-4F49-968F-328D3756EA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Shards</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,14 +88,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>相对基金方向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">买入
+卖出
+无操作
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000（0.5%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9000（0.6%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000（0.7%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11000（0.8%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前持仓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>历史持仓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对持仓百分比</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">买入
 卖出
@@ -108,52 +145,33 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Microsoft YaHei Light"/>
         <family val="2"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>保持</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>相对基金方向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">买入
-卖出
-无操作
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8000（0.5%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9000（0.6%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10000（0.7%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11000（0.8%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>当前持仓</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>历史持仓</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>相对持仓百分比</t>
+    <t>CUSIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXAMPLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88160R101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>”TESLA INC“</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -164,33 +182,31 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="3"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="3"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,30 +235,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,7 +274,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,138 +570,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EB39C5-F66E-4865-A96F-E3BCE74C61CA}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="3">
+        <v>44248</v>
+      </c>
+      <c r="K2" s="3">
+        <v>44249</v>
+      </c>
+      <c r="L2" s="3">
+        <v>44250</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="99" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="3">
-        <v>44248</v>
-      </c>
-      <c r="I2" s="3">
-        <v>44249</v>
-      </c>
-      <c r="J2" s="3">
-        <v>44250</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>6</v>
+      <c r="G3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="96" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:J1"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>